<commit_message>
Modificaciones en el formato de la fecha y se añadio cierre de sesion
</commit_message>
<xml_diff>
--- a/AppSolutions/Exportar/Informes.xlsx
+++ b/AppSolutions/Exportar/Informes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t>Vehículo</x:t>
   </x:si>
@@ -37,31 +37,19 @@
     <x:t>Fecha de entrega</x:t>
   </x:si>
   <x:si>
-    <x:t>FME345</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MATHIAS SOTO BARBOSA</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> CEMENTO, VIGAS 6X4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ANTIOQUIA / ANGELOPOLIS    -    SANTANDER / CALIFORNIA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$4.885.200.000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FME444</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SANTIAGO BARRIENTOS</x:t>
+    <x:t>FMG399</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PEDRO PEREZ</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> CEMENTO, LADRILLOS</x:t>
   </x:si>
   <x:si>
-    <x:t>$3.776.000.000</x:t>
+    <x:t>SANTANDER / BUCARAMANGA    -    ANTIOQUIA / MEDELLIN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$24.454.400.000</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -132,8 +120,8 @@
 </file>
 
 <file path=xl/tables/table.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0">
-  <x:autoFilter ref="A1:G3"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G2" totalsRowShown="0">
+  <x:autoFilter ref="A1:G2"/>
   <x:tableColumns count="7">
     <x:tableColumn id="1" name="Vehículo"/>
     <x:tableColumn id="2" name="Persona a cargo"/>
@@ -435,15 +423,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G3"/>
+  <x:dimension ref="A1:G2"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="10.550625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="25.130625000000002" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="22.130625000000002" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="16.700625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="22.410625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="54.550625000000004" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="20.410625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="16.410625" style="0" customWidth="1"/>
@@ -490,33 +478,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F2" s="1">
-        <x:v>44936.4831361111</x:v>
+        <x:v>44943.7729996875</x:v>
       </x:c>
       <x:c r="G2" s="1">
-        <x:v>44936.4831361111</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="A3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="F3" s="1">
-        <x:v>44936.4824440972</x:v>
-      </x:c>
-      <x:c r="G3" s="1">
-        <x:v>44936.4824440972</x:v>
+        <x:v>44943.773196331</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>